<commit_message>
Correction plan de tests
</commit_message>
<xml_diff>
--- a/P5_02_plantests.xlsx
+++ b/P5_02_plantests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oremi\Documents\OpenClassroom\Projet 5\P5_omar_remina\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oremi\Documents\OpenClassroom\Projet 5\ReminaOmar_5_06072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239BFA57-AEA1-42BF-8AA1-50DFD4DF57FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ED5C7F-3753-4D70-8E7D-D3FB1AF6733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C60B831-8D2A-496B-B8A6-EA376D9A377C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>PLAN DE TESTS</t>
   </si>
@@ -66,13 +66,7 @@
     <t>Cliquer sur l'image d'un produit.</t>
   </si>
   <si>
-    <t>La page "Ma sélection" comprenant le produit sélectionné s'affiche.</t>
-  </si>
-  <si>
     <t>Cliquer sur "Accueil".</t>
-  </si>
-  <si>
-    <t>Cliquer le nom d'un produit.</t>
   </si>
   <si>
     <t>Cliquer sur la liste comprenant les couleurs.</t>
@@ -566,63 +560,12 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -630,12 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,6 +580,63 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -693,7 +687,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91F7986B-6C2A-49C0-94C4-AD5C9CFC81F6}" name="Tableau1" displayName="Tableau1" ref="A5:E31" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91F7986B-6C2A-49C0-94C4-AD5C9CFC81F6}" name="Tableau1" displayName="Tableau1" ref="A5:E30" totalsRowShown="0" dataDxfId="8">
   <tableColumns count="5">
     <tableColumn id="5" xr3:uid="{2E0A60A4-8491-4B98-853F-C54DA94733F8}" name="Etapes" dataDxfId="7"/>
     <tableColumn id="1" xr3:uid="{5795D028-21D2-48DB-825F-E8D67B2407C3}" name="Action(s)" dataDxfId="6"/>
@@ -1026,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF0D3A-905A-4BAC-8CE7-7520DE2463BC}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,20 +1035,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1094,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1104,7 +1098,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1117,10 +1111,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1130,10 +1124,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1143,36 +1137,36 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1185,20 +1179,20 @@
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1208,15 +1202,15 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1229,15 +1223,15 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1247,10 +1241,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1260,23 +1254,23 @@
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1286,10 +1280,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1299,10 +1293,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1312,10 +1306,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1325,10 +1319,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1338,36 +1332,36 @@
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1377,7 +1371,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>82</v>
@@ -1385,52 +1379,39 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A32:E33"/>
+    <mergeCell ref="A31:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1443,7 +1424,7 @@
           <x14:formula1>
             <xm:f>Feuil4!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D31</xm:sqref>
+          <xm:sqref>D6:D30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1463,89 +1444,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="16">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4">
         <v>29</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <f>Tableau2[[#This Row],[Prix unitaire]]*Tableau2[[#This Row],[Quantité]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="16">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4">
         <v>39</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18">
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
         <f>Tableau2[[#This Row],[Prix unitaire]]*Tableau2[[#This Row],[Quantité]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="16">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4">
         <v>59</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6">
         <f>Tableau2[[#This Row],[Prix unitaire]]*Tableau2[[#This Row],[Quantité]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="16">
+        <v>46</v>
+      </c>
+      <c r="B5" s="4">
         <v>45</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6">
         <f>Tableau2[[#This Row],[Prix unitaire]]*Tableau2[[#This Row],[Quantité]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="16">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4">
         <v>55</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6">
         <f>Tableau2[[#This Row],[Prix unitaire]]*Tableau2[[#This Row],[Quantité]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="19">
+        <v>48</v>
+      </c>
+      <c r="D7" s="7">
         <f>SUM(D2:D6)</f>
         <v>0</v>
       </c>
@@ -1575,185 +1556,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="29"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="32"/>
-    </row>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="32"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C6" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="12">
+        <v>54545</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="C11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="29">
-        <v>54545</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="27" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="27" t="s">
-        <v>70</v>
+      <c r="C13" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="31"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="31"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="27" t="s">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="C19" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="C22" s="29"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="24"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C25" s="12">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="27" t="s">
+      <c r="C26" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="29">
-        <v>45454</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="C27" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1795,22 +1776,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification du plan de tests
</commit_message>
<xml_diff>
--- a/P5_02_plantests.xlsx
+++ b/P5_02_plantests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oremi\Documents\OpenClassroom\Projet 5\ReminaOmar_5_06072021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ED5C7F-3753-4D70-8E7D-D3FB1AF6733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96D8DB4-2FD8-438B-A8D3-C992EE4A96C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C60B831-8D2A-496B-B8A6-EA376D9A377C}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>FIN DES TESTS</t>
   </si>
   <si>
-    <t>Cliquer sur "ORINOCO" (en haut à gauche).</t>
-  </si>
-  <si>
     <t>La page "Mon nounours" comprenant le produit sélectionné s'affiche.</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Un message indiquant que le panier est vide doit apparaitre.</t>
+  </si>
+  <si>
+    <t>Cliquer sur "ORINOUNOURS" (en haut à gauche).</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A30"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1111,7 +1111,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1137,10 +1137,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1163,10 +1163,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1176,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -1192,7 +1192,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1228,10 +1228,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1244,7 +1244,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1257,7 +1257,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1270,7 +1270,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1296,7 +1296,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1309,7 +1309,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1322,7 +1322,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1335,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1348,7 +1348,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1361,7 +1361,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1371,10 +1371,10 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1387,7 +1387,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1444,21 +1444,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>29</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4">
         <v>39</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4">
         <v>59</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4">
         <v>45</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4">
         <v>55</v>
@@ -1524,7 +1524,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="7">
         <f>SUM(D2:D6)</f>
@@ -1557,7 +1557,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="15"/>
@@ -1571,37 +1571,37 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="12">
         <v>54545</v>
@@ -1609,36 +1609,36 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1647,75 +1647,75 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="31"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="29"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="12">
         <v>45454</v>
@@ -1723,18 +1723,18 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1776,22 +1776,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>